<commit_message>
adding a list of books + sql insert statements
</commit_message>
<xml_diff>
--- a/Books.xlsx
+++ b/Books.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\POJOH\Documents\bookstoreproject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DFB6B6-A177-49CF-B129-B9D628406796}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEE40C7-F7F6-434F-BB84-B03EC9D6FBAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{F603FC08-E058-4F14-914E-17A62F8B547B}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{F603FC08-E058-4F14-914E-17A62F8B547B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="305">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="306">
   <si>
     <t>Title</t>
   </si>
@@ -948,13 +948,16 @@
   </si>
   <si>
     <t>June 23, 2016</t>
+  </si>
+  <si>
+    <t>Database insert</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -967,6 +970,12 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF0033B3"/>
+      <name val="JetBrains Mono"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -989,9 +998,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1306,13 +1318,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C93772F4-DC4E-43D6-B45B-EE2DA20981A3}">
-  <dimension ref="A1:F101"/>
+  <dimension ref="A1:L101"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G2" sqref="G2:G101"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="44.7109375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="27.85546875" bestFit="1" customWidth="1"/>
@@ -1321,7 +1333,7 @@
     <col min="6" max="6" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1340,8 +1352,11 @@
       <c r="F1" t="s">
         <v>203</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
         <v>83</v>
       </c>
@@ -1361,8 +1376,12 @@
       <c r="F2" s="1" t="s">
         <v>206</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="str">
+        <f>_xlfn.CONCAT("INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('",A2,"','",B2,"','",E2,"','",F2,"'",")")</f>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Allt går sönder ','Chinua Achebe','2212.47','August 25, 1914')</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
       <c r="A3" t="s">
         <v>84</v>
       </c>
@@ -1382,8 +1401,12 @@
       <c r="F3" s="1" t="s">
         <v>207</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3" t="str">
+        <f t="shared" ref="G3:G66" si="1">_xlfn.CONCAT("INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('",A3,"','",B3,"','",E3,"','",F3,"'",")")</f>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Drottningens juvelsmycke','Carl Jonas Love Almqvist','412.6','May 18, 1927')</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
       <c r="A4" t="s">
         <v>85</v>
       </c>
@@ -1403,8 +1426,13 @@
       <c r="F4" s="1" t="s">
         <v>208</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Andarnas hus +','Isabel Allende','1320.24','December 31, 1927')</v>
+      </c>
+      <c r="L4" s="2"/>
+    </row>
+    <row r="5" spans="1:12">
       <c r="A5" t="s">
         <v>86</v>
       </c>
@@ -1424,8 +1452,13 @@
       <c r="F5" s="1" t="s">
         <v>209</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Ditte människobarn','Martin Andersen Nexö','1289.18','April 22, 1934')</v>
+      </c>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
         <v>87</v>
       </c>
@@ -1445,8 +1478,13 @@
       <c r="F6" s="1" t="s">
         <v>210</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Hitom himlen','Stina Aronson','1186.11','July 17, 1940')</v>
+      </c>
+      <c r="L6" s="2"/>
+    </row>
+    <row r="7" spans="1:12">
       <c r="A7" t="s">
         <v>88</v>
       </c>
@@ -1466,8 +1504,12 @@
       <c r="F7" s="1" t="s">
         <v>211</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Stolthet och fördom ','Jane Austen','1244.99','February 26, 1941')</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
       <c r="A8" t="s">
         <v>89</v>
       </c>
@@ -1487,8 +1529,12 @@
       <c r="F8" s="1" t="s">
         <v>212</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Pappa Goriot ','Honoré de Balzac','1804.21','September 29, 1941')</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
       <c r="A9" t="s">
         <v>90</v>
       </c>
@@ -1508,8 +1554,12 @@
       <c r="F9" s="1" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Ondskans blommor','Charles Baudelaire','827.25','February 9, 1943')</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
       <c r="A10" t="s">
         <v>91</v>
       </c>
@@ -1529,8 +1579,12 @@
       <c r="F10" s="1" t="s">
         <v>214</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('I väntan på Godot+','Samuel Beckett','1013.1','March 16, 1948')</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11" t="s">
         <v>92</v>
       </c>
@@ -1550,8 +1604,12 @@
       <c r="F11" s="1" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Onkel Toms stuga',' Harriet Beecher Stowe','1860.9','December 31, 1948')</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12" t="s">
         <v>93</v>
       </c>
@@ -1571,8 +1629,12 @@
       <c r="F12" s="1" t="s">
         <v>216</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Fru Marianne ',' Victoria Benedictsson','1673.48','March 14, 1951')</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13" t="s">
         <v>94</v>
       </c>
@@ -1592,8 +1654,12 @@
       <c r="F13" s="1" t="s">
         <v>217</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Röde Orm',' Frans G. Bengtsson','213.49','May 16, 1956')</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14" t="s">
         <v>95</v>
       </c>
@@ -1613,8 +1679,12 @@
       <c r="F14" s="1" t="s">
         <v>218</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Markurells i Wadköping (sett en teaterföreställn',' Hjalmar Bergman','2174.14','November 9, 1964')</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15" t="s">
         <v>96</v>
       </c>
@@ -1634,8 +1704,12 @@
       <c r="F15" s="1" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Decamerone',' Giovanni Boccaccio','938.58','May 30, 1969')</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16" t="s">
         <v>97</v>
       </c>
@@ -1655,8 +1729,12 @@
       <c r="F16" s="1" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Kallocain ',' Karin Boye','1969.16','June 28, 1970')</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" t="s">
         <v>98</v>
       </c>
@@ -1676,8 +1754,12 @@
       <c r="F17" s="1" t="s">
         <v>221</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Mor Courage och hennes barn',' Bertholt Brecht','1226.96','September 10, 1972')</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" t="s">
         <v>99</v>
       </c>
@@ -1697,8 +1779,12 @@
       <c r="F18" s="1" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Hertha',' Fredrika Bremer','1182.1','November 25, 1974')</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" t="s">
         <v>100</v>
       </c>
@@ -1718,8 +1804,12 @@
       <c r="F19" s="1" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Agnes Grey',' Anne Brontë','1611.15','October 25, 1976')</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" t="s">
         <v>101</v>
       </c>
@@ -1739,8 +1829,12 @@
       <c r="F20" s="1" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Jane Eyre ',' Charlotte Brontë','2483.79','November 11, 1985')</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" t="s">
         <v>102</v>
       </c>
@@ -1760,8 +1854,12 @@
       <c r="F21" s="1" t="s">
         <v>225</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Svindlande höjder',' Emily Brontë','1478.33','February 12, 2005')</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" t="s">
         <v>103</v>
       </c>
@@ -1781,8 +1879,12 @@
       <c r="F22" s="1" t="s">
         <v>226</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Mästaren och Margarita',' Mikhail Bulgakov','1437.93','November 23, 2013')</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" t="s">
         <v>104</v>
       </c>
@@ -1802,8 +1904,12 @@
       <c r="F23" s="1" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Om en vinternatt en resande *',' Italo Calvino','2149.59','October 8, 2014')</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
       <c r="A24" t="s">
         <v>105</v>
       </c>
@@ -1823,8 +1929,12 @@
       <c r="F24" s="1" t="s">
         <v>228</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Främlingen +',' Albert Camus','1879.74','March 8, 2015')</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
       <c r="A25" t="s">
         <v>106</v>
       </c>
@@ -1844,8 +1954,12 @@
       <c r="F25" s="1" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Drömmar om röda gemak',' Cao Xueqin','988.19','March 17, 2015')</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
       <c r="A26" t="s">
         <v>107</v>
       </c>
@@ -1865,8 +1979,12 @@
       <c r="F26" s="1" t="s">
         <v>230</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Don Quijote',' Cervantes','2220.61','May 27, 2016')</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
       <c r="A27" t="s">
         <v>108</v>
       </c>
@@ -1886,8 +2004,12 @@
       <c r="F27" s="1" t="s">
         <v>231</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Mörkrets hjärta',' Joseph Conrad','1976.74','April 12, 1922')</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
       <c r="A28" t="s">
         <v>109</v>
       </c>
@@ -1907,8 +2029,12 @@
       <c r="F28" s="1" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Den gudomliga komedin',' Dante Alighieri','2469.78','June 13, 1927')</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
       <c r="A29" t="s">
         <v>110</v>
       </c>
@@ -1928,8 +2054,12 @@
       <c r="F29" s="1" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Robinson Crusoe ',' Daniel Defoe','2238.14','December 10, 1927')</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" t="s">
         <v>111</v>
       </c>
@@ -1949,8 +2079,12 @@
       <c r="F30" s="1" t="s">
         <v>234</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Oliver Twist ',' Charles Dickens','2318.39','October 6, 1929')</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
       <c r="A31" t="s">
         <v>112</v>
       </c>
@@ -1970,8 +2104,12 @@
       <c r="F31" s="1" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Brott och straff +',' Fjodor Dostojevskij','2298.18','July 18, 1931')</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
       <c r="A32" t="s">
         <v>113</v>
       </c>
@@ -1991,8 +2129,12 @@
       <c r="F32" s="1" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('De tre musketörerna ',' Alexandre Dumas d ä','1479.45','July 6, 1935')</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
       <c r="A33" t="s">
         <v>114</v>
       </c>
@@ -2012,8 +2154,12 @@
       <c r="F33" s="1" t="s">
         <v>237</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G33" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Älskaren +',' Marguerite Duras','1611.73','July 14, 1939')</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
       <c r="A34" t="s">
         <v>115</v>
       </c>
@@ -2033,8 +2179,12 @@
       <c r="F34" s="1" t="s">
         <v>238</v>
       </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G34" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Det öde landet+',' T S Eliot','533.14','August 7, 1940')</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
       <c r="A35" t="s">
         <v>116</v>
       </c>
@@ -2054,8 +2204,12 @@
       <c r="F35" s="1" t="s">
         <v>239</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G35" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Medea+',' Euripides','2390.12','July 11, 1946')</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
       <c r="A36" t="s">
         <v>117</v>
       </c>
@@ -2075,8 +2229,12 @@
       <c r="F36" s="1" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G36" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Absalom, Absalom',' William Faulkner','1411.26','September 20, 1955')</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
       <c r="A37" t="s">
         <v>118</v>
       </c>
@@ -2096,8 +2254,12 @@
       <c r="F37" s="1" t="s">
         <v>241</v>
       </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G37" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Den store Gatsby+',' F Scott Fitzgerald','857.89','July 26, 1956')</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
       <c r="A38" t="s">
         <v>119</v>
       </c>
@@ -2117,8 +2279,12 @@
       <c r="F38" s="1" t="s">
         <v>242</v>
       </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G38" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Madame Bovary',' Gustave Flaubert','1582.75','September 15, 1957')</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
       <c r="A39" t="s">
         <v>120</v>
       </c>
@@ -2138,8 +2304,12 @@
       <c r="F39" s="1" t="s">
         <v>243</v>
       </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G39" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Rosen på Tistelön',' Emilie Flygare-Carlén','1796.90','November 28, 1962')</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
       <c r="A40" t="s">
         <v>121</v>
       </c>
@@ -2159,8 +2329,12 @@
       <c r="F40" s="1" t="s">
         <v>244</v>
       </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G40" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Stockholms-serien +',' Per Anders Fogelström','309.82','June 28, 1964')</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
       <c r="A41" t="s">
         <v>122</v>
       </c>
@@ -2180,8 +2354,12 @@
       <c r="F41" s="1" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G41" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Hundra år av ensamhet +',' Gabriel García Márquez','2100.28','November 30, 1967')</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7">
       <c r="A42" t="s">
         <v>123</v>
       </c>
@@ -2201,8 +2379,12 @@
       <c r="F42" s="1" t="s">
         <v>246</v>
       </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G42" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Den omoraliske',' André Gide','1453.24','June 7, 1968')</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
       <c r="A43" t="s">
         <v>124</v>
       </c>
@@ -2222,8 +2404,12 @@
       <c r="F43" s="1" t="s">
         <v>247</v>
       </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G43" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Den unge Werthers lidanden ',' Johann Wolfgang von Goethe','1185.14','October 6, 1989')</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
       <c r="A44" t="s">
         <v>125</v>
       </c>
@@ -2243,8 +2429,12 @@
       <c r="F44" s="1" t="s">
         <v>248</v>
       </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G44" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Min barndom',' Maksim Gorkij','459.68','January 20, 1996')</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7">
       <c r="A45" t="s">
         <v>126</v>
       </c>
@@ -2264,8 +2454,12 @@
       <c r="F45" s="1" t="s">
         <v>249</v>
       </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G45" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Brighton Rock',' Graham Greene','2250.20','June 25, 1999')</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7">
       <c r="A46" t="s">
         <v>127</v>
       </c>
@@ -2285,8 +2479,12 @@
       <c r="F46" s="1" t="s">
         <v>250</v>
       </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G46" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Markens gröda',' Knut Hamsun','1308.88','April 21, 2002')</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7">
       <c r="A47" t="s">
         <v>128</v>
       </c>
@@ -2306,8 +2504,12 @@
       <c r="F47" s="1" t="s">
         <v>251</v>
       </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G47" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Den tappre soldaten Svejk',' Jaroslav Hasek','1813.10','September 13, 2010')</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7">
       <c r="A48" t="s">
         <v>129</v>
       </c>
@@ -2327,8 +2529,12 @@
       <c r="F48" s="1" t="s">
         <v>252</v>
       </c>
-    </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G48" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Moment 22',' Joseph Heller','324.92','February 9, 2011')</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7">
       <c r="A49" t="s">
         <v>130</v>
       </c>
@@ -2348,8 +2554,12 @@
       <c r="F49" s="1" t="s">
         <v>253</v>
       </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G49" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Den gamle och havet ',' Ernest Hemingway','2285.30','February 13, 2012')</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7">
       <c r="A50" t="s">
         <v>131</v>
       </c>
@@ -2369,8 +2579,12 @@
       <c r="F50" s="1" t="s">
         <v>254</v>
       </c>
-    </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G50" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Stäppvargen?',' Hermann Hesse','2161.68','December 3, 2013')</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7">
       <c r="A51" t="s">
         <v>132</v>
       </c>
@@ -2390,8 +2604,12 @@
       <c r="F51" s="1" t="s">
         <v>255</v>
       </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G51" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Odysséen',' Homeros','2441.33','March 28, 2014')</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7">
       <c r="A52" t="s">
         <v>133</v>
       </c>
@@ -2411,8 +2629,12 @@
       <c r="F52" s="1" t="s">
         <v>256</v>
       </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G52" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Et dukkehjem',' Henrik Ibsen','623.92','October 17, 1921')</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7">
       <c r="A53" t="s">
         <v>134</v>
       </c>
@@ -2432,8 +2654,12 @@
       <c r="F53" s="1" t="s">
         <v>257</v>
       </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G53" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Strändernas svall',' Eyvind Johnson','975.62','May 31, 1922')</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7">
       <c r="A54" t="s">
         <v>135</v>
       </c>
@@ -2453,8 +2679,12 @@
       <c r="F54" s="1" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G54" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Ulysses',' James Joyce','1473.45','May 30, 1926')</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7">
       <c r="A55" t="s">
         <v>136</v>
       </c>
@@ -2474,8 +2704,12 @@
       <c r="F55" s="1" t="s">
         <v>259</v>
       </c>
-    </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G55" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Processen ',' Franz Kafka','1061.5','December 29, 1927')</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7">
       <c r="A56" t="s">
         <v>137</v>
       </c>
@@ -2495,8 +2729,12 @@
       <c r="F56" s="1" t="s">
         <v>260</v>
       </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G56" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Låt tistlarna brinna!',' Yasar Kemal','856.13','November 4, 1930')</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7">
       <c r="A57" t="s">
         <v>138</v>
       </c>
@@ -2516,8 +2754,12 @@
       <c r="F57" s="1" t="s">
         <v>261</v>
       </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G57" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Bertha Funke*',' Kleve, Stella (Malling, Math','1678.59','October 25, 1935')</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7">
       <c r="A58" t="s">
         <v>139</v>
       </c>
@@ -2537,8 +2779,12 @@
       <c r="F58" s="1" t="s">
         <v>262</v>
       </c>
-    </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G58" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Barabbas +',' Pär Lagerkvist','1516.20','April 10, 1941')</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7">
       <c r="A59" t="s">
         <v>140</v>
       </c>
@@ -2558,8 +2804,12 @@
       <c r="F59" s="1" t="s">
         <v>263</v>
       </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G59" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Kejsarn av Portugallien ',' Selma Lagerlöf','1652.24','September 30, 1941')</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7">
       <c r="A60" t="s">
         <v>141</v>
       </c>
@@ -2579,8 +2829,12 @@
       <c r="F60" s="1" t="s">
         <v>264</v>
       </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G60" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Lifsens rot',' Lidman, Sara','1395.19','February 7, 1944')</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7">
       <c r="A61" t="s">
         <v>142</v>
       </c>
@@ -2600,8 +2854,12 @@
       <c r="F61" s="1" t="s">
         <v>265</v>
       </c>
-    </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G61" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Okänd soldat (har läst utdrag, räknas det?)',' Väinö Linna','1128.33','March 29, 1959')</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7">
       <c r="A62" t="s">
         <v>143</v>
       </c>
@@ -2621,8 +2879,12 @@
       <c r="F62" s="1" t="s">
         <v>266</v>
       </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G62" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Kungsgatan',' Ivar Lo-Johansson','603.87','December 23, 1963')</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7">
       <c r="A63" t="s">
         <v>144</v>
       </c>
@@ -2642,8 +2904,12 @@
       <c r="F63" s="1" t="s">
         <v>245</v>
       </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G63" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Huset Buddenbrook',' Thomas Mann','1389.89','November 30, 1967')</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7">
       <c r="A64" t="s">
         <v>145</v>
       </c>
@@ -2663,8 +2929,12 @@
       <c r="F64" s="1" t="s">
         <v>267</v>
       </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G64" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Nässlorna blomma',' Harry Martinson','515.86','July 19, 1968')</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7">
       <c r="A65" t="s">
         <v>146</v>
       </c>
@@ -2684,8 +2954,12 @@
       <c r="F65" s="1" t="s">
         <v>268</v>
       </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G65" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Kvinnor och äppelträd',' Moa Martinson','276.66','October 28, 1976')</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7">
       <c r="A66" t="s">
         <v>147</v>
       </c>
@@ -2705,8 +2979,12 @@
       <c r="F66" s="1" t="s">
         <v>269</v>
       </c>
-    </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G66" t="str">
+        <f t="shared" si="1"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Utvandrar-serien',' Vilhelm Moberg','1353.11','March 27, 1977')</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7">
       <c r="A67" t="s">
         <v>148</v>
       </c>
@@ -2720,14 +2998,18 @@
         <v>64</v>
       </c>
       <c r="E67" t="str">
-        <f t="shared" ref="E67:E101" si="1">_xlfn.CONCAT(C67,".",D67)</f>
+        <f t="shared" ref="E67:E101" si="2">_xlfn.CONCAT(C67,".",D67)</f>
         <v>907.64</v>
       </c>
       <c r="F67" s="1" t="s">
         <v>270</v>
       </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G67" t="str">
+        <f t="shared" ref="G67:G101" si="3">_xlfn.CONCAT("INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('",A67,"','",B67,"','",E67,"','",F67,"'",")")</f>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Tartuffe',' Molière','907.64','September 13, 1981')</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7">
       <c r="A68" t="s">
         <v>149</v>
       </c>
@@ -2741,14 +3023,18 @@
         <v>71</v>
       </c>
       <c r="E68" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1740.71</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>271</v>
       </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G68" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Historien*',' Elsa Morante','1740.71','May 9, 1993')</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7">
       <c r="A69" t="s">
         <v>150</v>
       </c>
@@ -2762,14 +3048,18 @@
         <v>83</v>
       </c>
       <c r="E69" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>863.83</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>272</v>
       </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G69" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Älskade ',' Morrison, Toni','863.83','January 23, 1995')</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7">
       <c r="A70" t="s">
         <v>151</v>
       </c>
@@ -2783,14 +3073,18 @@
         <v>4</v>
       </c>
       <c r="E70" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2289.4</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>273</v>
       </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G70" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Lolita',' Vladimir Nabokov','2289.4','February 3, 1995')</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7">
       <c r="A71" t="s">
         <v>152</v>
       </c>
@@ -2804,14 +3098,18 @@
         <v>94</v>
       </c>
       <c r="E71" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>439.94</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>274</v>
       </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G71" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('1984 +',' George Orwell','439.94','April 16, 1998')</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7">
       <c r="A72" t="s">
         <v>153</v>
       </c>
@@ -2825,14 +3123,18 @@
         <v>20</v>
       </c>
       <c r="E72" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>719.20</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>275</v>
       </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G72" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Doktor Zjivago',' Boris Pasternak','719.20','May 30, 1998')</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7">
       <c r="A73" t="s">
         <v>154</v>
       </c>
@@ -2846,14 +3148,18 @@
         <v>61</v>
       </c>
       <c r="E73" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1543.61</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>276</v>
       </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G73" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Kärleksdikter',' Francesco Petrarca','1543.61','October 11, 2001')</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7">
       <c r="A74" t="s">
         <v>155</v>
       </c>
@@ -2867,14 +3173,18 @@
         <v>35</v>
       </c>
       <c r="E74" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2170.35</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>277</v>
       </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G74" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('På spaning efter den tid som flytt ',' Marcel Proust','2170.35','April 3, 2004')</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7">
       <c r="A75" t="s">
         <v>156</v>
       </c>
@@ -2888,14 +3198,18 @@
         <v>23</v>
       </c>
       <c r="E75" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1937.23</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>278</v>
       </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G75" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('På Västfronten intet nytt ',' Erich Maria Remarque','1937.23','November 13, 2016')</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7">
       <c r="A76" t="s">
         <v>157</v>
       </c>
@@ -2909,14 +3223,18 @@
         <v>86</v>
       </c>
       <c r="E76" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2094.86</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>279</v>
       </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G76" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Räddaren i nöden',' J. D. Salinger','2094.86','August 13, 2018')</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7">
       <c r="A77" t="s">
         <v>158</v>
       </c>
@@ -2930,14 +3248,18 @@
         <v>76</v>
       </c>
       <c r="E77" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2282.76</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G77" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Alberte-serien x läst första delen i serien.',' Cora Sandel','2282.76','June 27, 1914')</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7">
       <c r="A78" t="s">
         <v>159</v>
       </c>
@@ -2951,14 +3273,18 @@
         <v>27</v>
       </c>
       <c r="E78" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>234.27</v>
       </c>
       <c r="F78" s="1" t="s">
         <v>281</v>
       </c>
-    </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G78" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Dikter och fragment',' Sapfo','234.27','November 6, 1917')</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7">
       <c r="A79" t="s">
         <v>160</v>
       </c>
@@ -2972,14 +3298,18 @@
         <v>41</v>
       </c>
       <c r="E79" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>344.41</v>
       </c>
       <c r="F79" s="1" t="s">
         <v>282</v>
       </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G79" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Macbeth+',' William Shakespeare','344.41','August 2, 1921')</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7">
       <c r="A80" t="s">
         <v>161</v>
       </c>
@@ -2993,14 +3323,18 @@
         <v>81</v>
       </c>
       <c r="E80" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1103.81</v>
       </c>
       <c r="F80" s="1" t="s">
         <v>283</v>
       </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G80" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Frankenstein ',' Mary Shelley','1103.81','October 31, 1921')</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7">
       <c r="A81" t="s">
         <v>162</v>
       </c>
@@ -3014,14 +3348,18 @@
         <v>69</v>
       </c>
       <c r="E81" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2092.69</v>
       </c>
       <c r="F81" s="1" t="s">
         <v>284</v>
       </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G81" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Konung Oidipus',' Sofokles','2092.69','October 13, 1922')</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7">
       <c r="A82" t="s">
         <v>163</v>
       </c>
@@ -3035,14 +3373,18 @@
         <v>67</v>
       </c>
       <c r="E82" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2078.67</v>
       </c>
       <c r="F82" s="1" t="s">
         <v>285</v>
       </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G82" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('En dag i Ivan Denisovitjs liv ',' Solzjenitsyn','2078.67','July 20, 1930')</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7">
       <c r="A83" t="s">
         <v>164</v>
       </c>
@@ -3056,14 +3398,18 @@
         <v>83</v>
       </c>
       <c r="E83" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1948.83</v>
       </c>
       <c r="F83" s="1" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G83" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Vredens druvor',' John Steinbeck','1948.83','April 3, 1936')</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7">
       <c r="A84" t="s">
         <v>165</v>
       </c>
@@ -3077,14 +3423,18 @@
         <v>47</v>
       </c>
       <c r="E84" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2439.47</v>
       </c>
       <c r="F84" s="1" t="s">
         <v>287</v>
       </c>
-    </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G84" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Rött och svart*',' Stendhal','2439.47','January 12, 1942')</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7">
       <c r="A85" t="s">
         <v>166</v>
       </c>
@@ -3098,14 +3448,18 @@
         <v>97</v>
       </c>
       <c r="E85" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1318.97</v>
       </c>
       <c r="F85" s="1" t="s">
         <v>288</v>
       </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G85" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Dracula',' Bram Stoker','1318.97','January 12, 1943')</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7">
       <c r="A86" t="s">
         <v>167</v>
       </c>
@@ -3119,14 +3473,18 @@
         <v>6</v>
       </c>
       <c r="E86" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1400.6</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>289</v>
       </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G86" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Dr Jekyll och Mr Hyde',' Robert Louis Stevenson','1400.6','May 8, 1944')</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7">
       <c r="A87" t="s">
         <v>168</v>
       </c>
@@ -3140,14 +3498,18 @@
         <v>70</v>
       </c>
       <c r="E87" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>671.70</v>
       </c>
       <c r="F87" s="1" t="s">
         <v>290</v>
       </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G87" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Röda rummet',' August Strindberg','671.70','January 24, 1948')</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7">
       <c r="A88" t="s">
         <v>169</v>
       </c>
@@ -3161,14 +3523,18 @@
         <v>75</v>
       </c>
       <c r="E88" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>213.75</v>
       </c>
       <c r="F88" s="1" t="s">
         <v>291</v>
       </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G88" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Egil Skallagrimssons saga',' Snorre Sturlasson (?)','213.75','September 16, 1951')</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7">
       <c r="A89" t="s">
         <v>170</v>
       </c>
@@ -3182,14 +3548,18 @@
         <v>12</v>
       </c>
       <c r="E89" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1187.12</v>
       </c>
       <c r="F89" s="1" t="s">
         <v>292</v>
       </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G89" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Gullivers resor',' Jonathan Swift','1187.12','April 29, 1955')</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7">
       <c r="A90" t="s">
         <v>171</v>
       </c>
@@ -3203,14 +3573,18 @@
         <v>62</v>
       </c>
       <c r="E90" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1094.62</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>293</v>
       </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G90" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Den allvarsamma leken +',' Hjalmar Söderberg','1094.62','January 3, 1958')</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7">
       <c r="A91" t="s">
         <v>172</v>
       </c>
@@ -3224,14 +3598,18 @@
         <v>58</v>
       </c>
       <c r="E91" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1898.58</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>294</v>
       </c>
-    </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G91" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Damen med hunden ',' Anton Tjechov','1898.58','October 23, 1958')</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7">
       <c r="A92" t="s">
         <v>173</v>
       </c>
@@ -3245,14 +3623,18 @@
         <v>47</v>
       </c>
       <c r="E92" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>796.47</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>295</v>
       </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G92" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Anna Karenina +',' Lev Tolstoj','796.47','February 27, 1965')</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7">
       <c r="A93" t="s">
         <v>174</v>
       </c>
@@ -3266,14 +3648,18 @@
         <v>50</v>
       </c>
       <c r="E93" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1496.50</v>
       </c>
       <c r="F93" s="1" t="s">
         <v>296</v>
       </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G93" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Huckleberry Finn',' Mark Twain','1496.50','July 12, 1976')</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7">
       <c r="A94" t="s">
         <v>175</v>
       </c>
@@ -3287,14 +3673,18 @@
         <v>87</v>
       </c>
       <c r="E94" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>869.87</v>
       </c>
       <c r="F94" s="1" t="s">
         <v>297</v>
       </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G94" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Kristin Lavransdotter',' Sigrid Undset','869.87','August 7, 1978')</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7">
       <c r="A95" t="s">
         <v>176</v>
       </c>
@@ -3308,14 +3698,18 @@
         <v>14</v>
       </c>
       <c r="E95" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>554.14</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>298</v>
       </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G95" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Jorden runt på 80 dagar +',' Jules Verne','554.14','June 30, 1985')</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7">
       <c r="A96" t="s">
         <v>177</v>
       </c>
@@ -3329,14 +3723,18 @@
         <v>42</v>
       </c>
       <c r="E96" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2295.42</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>299</v>
       </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G96" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Candide ',' Voltaire','2295.42','April 24, 1986')</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7">
       <c r="A97" t="s">
         <v>178</v>
       </c>
@@ -3350,14 +3748,18 @@
         <v>75</v>
       </c>
       <c r="E97" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>815.75</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>300</v>
       </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G97" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Dorian Grays porträtt ',' Oscar Wilde','815.75','June 8, 1991')</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7">
       <c r="A98" t="s">
         <v>179</v>
       </c>
@@ -3371,14 +3773,18 @@
         <v>16</v>
       </c>
       <c r="E98" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>591.16</v>
       </c>
       <c r="F98" s="1" t="s">
         <v>301</v>
       </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G98" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Mot fyren',' Woolf, Virginia','591.16','April 14, 2002')</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7">
       <c r="A99" t="s">
         <v>180</v>
       </c>
@@ -3392,14 +3798,18 @@
         <v>2</v>
       </c>
       <c r="E99" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>980.2</v>
       </c>
       <c r="F99" s="1" t="s">
         <v>302</v>
       </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G99" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Pennskaftet',' Wägner, Elin','980.2','December 24, 2005')</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7">
       <c r="A100" t="s">
         <v>181</v>
       </c>
@@ -3413,14 +3823,18 @@
         <v>40</v>
       </c>
       <c r="E100" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1066.40</v>
       </c>
       <c r="F100" s="1" t="s">
         <v>303</v>
       </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G100" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Tornet',' William Butler Yeats','1066.40','December 20, 2007')</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7">
       <c r="A101" t="s">
         <v>182</v>
       </c>
@@ -3434,11 +3848,15 @@
         <v>89</v>
       </c>
       <c r="E101" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1483.89</v>
       </c>
       <c r="F101" s="1" t="s">
         <v>304</v>
+      </c>
+      <c r="G101" t="str">
+        <f t="shared" si="3"/>
+        <v>INSERT INTO BOOK (TITLE, AUTHOR, PRICE, DATE) VALUES ('Thérèse Raquin','Émile Zola','1483.89','June 23, 2016')</v>
       </c>
     </row>
   </sheetData>

</xml_diff>